<commit_message>
Now using cython as default filter
</commit_message>
<xml_diff>
--- a/examples/excel_1.xlsx
+++ b/examples/excel_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source_code\COMSAFE\py_file_reader\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FB2C58-913F-4EEF-B444-5A760D8EDEB8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8B8DF5-D5AF-4050-902A-7DF1A809C884}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +607,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="3">
-        <v>43466</v>
+        <v>43101</v>
       </c>
       <c r="G12" s="3">
         <v>43257</v>
@@ -683,8 +683,11 @@
       <c r="D16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F16" s="3">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -697,8 +700,14 @@
       <c r="D17">
         <v>666</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="3">
+        <v>43466</v>
+      </c>
+      <c r="F17" s="3">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -712,7 +721,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>

</xml_diff>